<commit_message>
Boton descargar excel, Timeline Twitter, Likes facebook y Tw
</commit_message>
<xml_diff>
--- a/Twitter/df_tw.xlsx
+++ b/Twitter/df_tw.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hola! Espero que tengas un lindo día. Recuerda que eres amigable. Ejercitate para cuidarte y distraerte</t>
+          <t>AT_USER hola buenas tardes. Para reportar que en la colonia Independencia no hay servicio de electricidad. Calle Nu… https://t.co/jFONkB9JCH</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2.077134815734293</v>
+        <v>4.210312945518886</v>
       </c>
     </row>
     <row r="3">
@@ -482,8 +482,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RT AT_USER Hola Gem!, haz click en la puerta 
-                         🚪</t>
+          <t>AT_USER AT_USER AT_USER AT_USER AT_USER Hola galán...cuanta belleza en un solo ser😏😂</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -495,7 +494,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2.396117245484303</v>
+        <v>2.585497472318276</v>
       </c>
     </row>
     <row r="4">
@@ -504,7 +503,8 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Hola AT_USER dm</t>
+          <t>AT_USER AT_USER AT_USER ¡Hola AT_USER ! Quisiera que pasaran #SiTúNoEstás de AT_USER
+Ademá… https://t.co/efwJ648Fzx</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2.015138867859281</v>
+        <v>3.228837904625783</v>
       </c>
     </row>
     <row r="5">
@@ -525,7 +525,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AT_USER hola buen día, tengo una duda: defender la diversidad incluye cambiar el concepto de familia: padre, madre e hijos?</t>
+          <t>HOLA CHE</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.7517602189894903</v>
+        <v>1.790779697604845</v>
       </c>
     </row>
     <row r="6">
@@ -546,7 +546,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>RT AT_USER #CuentasClaras Hola amigos, al día de hoy en donaciones se han recibido $ 1,797.742 en nuestro perfil de Twitter está colgada…</t>
+          <t>AT_USER AT_USER HOLA, SIGO A TODOS.</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>5.743448832123979</v>
+        <v>2.152339989372766</v>
       </c>
     </row>
     <row r="7">
@@ -567,7 +567,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AT_USER Hola princesa bella buenos días disculpa me puedes seguir porfa gracias</t>
+          <t>AT_USER ¡Hola! En junio que llegue deberás descargar la app de HBO Max e iniciar sesión con tu usuario y contraseña, ¿emocionados? 🔥💜</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -579,7 +579,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>7.665194964341168</v>
+        <v>6.389042619053003</v>
       </c>
     </row>
     <row r="8">
@@ -588,7 +588,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RT AT_USER hola estoy bien (no estoy bien)</t>
+          <t>AT_USER AT_USER Hola AT_USER solicitamos verificar el caso que menciona el usuario… https://t.co/pNz0MlSiVF</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2.375914538166784</v>
+        <v>3.480798120788066</v>
       </c>
     </row>
     <row r="9">
@@ -609,7 +609,8 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RT AT_USER Hola AT_USER le hago una consulta: una fuente me informa que en el country San Carlos se han realizado vacunaciones…</t>
+          <t>AT_USER Me la quiero follar.
+Hola matz :3</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -621,7 +622,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>4.854669961909399</v>
+        <v>1.353537815812323</v>
       </c>
     </row>
     <row r="10">
@@ -630,7 +631,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AT_USER ¡ Hola Ramblings... Buenos días... Hermoso Mensaje... Felicidad y Bendiciones para TODOS ! https://t.co/dSP15RlasL</t>
+          <t>RT AT_USER Hola me gustan los gatitos :3</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -642,7 +643,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>6.46485366685696</v>
+        <v>2.701498895035485</v>
       </c>
     </row>
     <row r="11">
@@ -651,7 +652,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER AT_USER https://t.co/R2QB5kx91d</t>
+          <t>RT AT_USER hola AT_USER mira lo que hice, mi mamá me va a gritar 🙏 https://t.co/8HlezAhcwG</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -663,7 +664,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.6492423642197017</v>
+        <v>0.6878198641831308</v>
       </c>
     </row>
     <row r="12">
@@ -672,7 +673,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AT_USER Hola! Para poder entrar a COL debo tener pasaje de regreso a Chile?? Resido en Chile pero soy venezolano</t>
+          <t>AT_USER hola necesito saber el estado de un paquete urgente</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -684,7 +685,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1.70478700852815</v>
+        <v>2.80493042210277</v>
       </c>
     </row>
     <row r="13">
@@ -693,7 +694,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>RT AT_USER AT_USER Hola. Te paso info sobre cómo reclamar https://t.co/MSNqcvtDLW</t>
+          <t>AT_USER Hola,te invitamos a seguirnos 💗 somos un emprendimiento  que aca de iniciar estamos lleno de amor y sabe… https://t.co/MVJ0ayYrJw</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -705,7 +706,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2.954387831498278</v>
+        <v>5.308457611661656</v>
       </c>
     </row>
     <row r="14">
@@ -714,7 +715,8 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>AT_USER hola camii</t>
+          <t>RT AT_USER AT_USER Seis 
+Hola AT_USER me gustaría ver a AT_USER con una nominación o perfomance #PremiosMTVMiaw , gracia…</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -726,7 +728,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1.790779697604845</v>
+        <v>5.489783268886954</v>
       </c>
     </row>
     <row r="15">
@@ -735,7 +737,8 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>RT AT_USER Hola em dic Cristian, tinc 28 anys i busco feina per la zona de l'Alt Empordà a preferir de massatgista o jardiner però…</t>
+          <t>AT_USER AT_USER AT_USER ¡Hola AT_USER ! Quisiera que pasaran #SiTúNoEstás de AT_USER
+Ademá… https://t.co/OFL2DBktDC</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -747,7 +750,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.9854345887273618</v>
+        <v>3.228837904625783</v>
       </c>
     </row>
     <row r="16">
@@ -756,7 +759,10 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AT_USER "Hola Mundo!"</t>
+          <t>AT_USER Hola! Como estás? 
+Soy AT_USER de 🇦🇷🇦🇷
+Fan de danna García
+Te empecé a seguir en Twitter Quisiera q… https://t.co/2ChtLn3sro</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -768,7 +774,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>1.546204185802451</v>
+        <v>5.103481259972186</v>
       </c>
     </row>
     <row r="17">
@@ -777,7 +783,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>RT AT_USER #15May “Difundo Caracas 😭💔 "Hola  este perrito está ubicado en el bulevar la marrón, adyacente a la catedral quien pueda…</t>
+          <t>RT AT_USER Hola AT_USER porfavor si puedes difundir ese vídeo  es de una fundación de animales en Venezuela estado la Guaira y…</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -785,11 +791,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>-1.026512096666037</v>
+        <v>3.045177377357259</v>
       </c>
     </row>
     <row r="18">
@@ -798,9 +804,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RT AT_USER #Quevivanlasnovias14 
-Hola, se que ya no es 14 sorry.
-Hice este vídeo solo por qué estoy aburrido, espero que les guste.…</t>
+          <t>AT_USER Hola que tal sígueme para mandarte md</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -808,11 +812,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2.071823786948162</v>
+        <v>0.3465286669541487</v>
       </c>
     </row>
     <row r="19">
@@ -821,8 +825,8 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>RT AT_USER Hola Twitter.
-En Enero una tía fue diagnosticada con Carcimoma en seno izquierdo y requiere 3 ampollas de Placlitaxel 150m…</t>
+          <t>AT_USER 
+Hola</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -834,7 +838,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>3.073221591733438</v>
+        <v>1.790779697604845</v>
       </c>
     </row>
     <row r="20">
@@ -843,7 +847,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>hola buenos dias</t>
+          <t>AT_USER hola  papi hermoso</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -855,7 +859,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>2.73105220278663</v>
+        <v>3.312407977358458</v>
       </c>
     </row>
     <row r="21">
@@ -864,7 +868,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RT AT_USER Hola qué tal te vengo a ofrecer mi promoción , háblame por whatsapp: 2291313005 y realiza tu pedido , apóyenme con un rt, e…</t>
+          <t>RT AT_USER Hola Chicas Votamos 😊🙏❤
+Mavi-Sancar #SefirinKızı 
+👇👇👇👇👇👇👇👇👇
+https://t.co/ApDkzqCeXN
+#EnginAkyürek #TubaBüyüküstün https://t…</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -876,7 +884,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>3.305058415600876</v>
+        <v>2.238883743837056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>